<commit_message>
init project with data and metadata
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/GeoPressureTemplate/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Desktop/MK-RCRC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E82ECC3-1BB7-3A49-B25A-1ACE056F9CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A98335-90DE-2746-B947-C0E5EC4AB7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>mass</t>
   </si>
@@ -114,12 +114,6 @@
     <t>thr_dur</t>
   </si>
   <si>
-    <t>18LX</t>
-  </si>
-  <si>
-    <t>Great Reed Warbler</t>
-  </si>
-  <si>
     <t>thr_prob_percentile</t>
   </si>
   <si>
@@ -142,13 +136,55 @@
   </si>
   <si>
     <t>ringNo</t>
+  </si>
+  <si>
+    <t>24TA</t>
+  </si>
+  <si>
+    <t>27MN</t>
+  </si>
+  <si>
+    <t>27LH</t>
+  </si>
+  <si>
+    <t>25LQ</t>
+  </si>
+  <si>
+    <t>24SZ</t>
+  </si>
+  <si>
+    <t>24UL</t>
+  </si>
+  <si>
+    <t>24VC</t>
+  </si>
+  <si>
+    <t>Cossypha natalensis</t>
+  </si>
+  <si>
+    <t>Halcyon senegaloides</t>
+  </si>
+  <si>
+    <t>Red-capped Robin-Chat</t>
+  </si>
+  <si>
+    <t>Red-capped Robin-chat</t>
+  </si>
+  <si>
+    <t>Mangrove Kingfisher</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>multisensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,12 +332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFAD0000"/>
       <name val="Var(--bs-font-monospace)"/>
@@ -488,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -603,6 +633,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -649,13 +690,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -702,48 +744,328 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -761,8 +1083,14 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="22"/>
         </left>
@@ -775,8 +1103,6 @@
         <bottom style="thin">
           <color indexed="22"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -793,44 +1119,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AI2" totalsRowShown="0">
-  <autoFilter ref="A1:AI2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
-  <tableColumns count="35">
-    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="14" dataCellStyle="Normal_Feuil1"/>
-    <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start"/>
-    <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end"/>
-    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="13"/>
-    <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N"/>
-    <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W"/>
-    <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S"/>
-    <tableColumn id="46" xr3:uid="{4736E547-D326-6746-9382-CDD964418C71}" name="extent_E"/>
-    <tableColumn id="47" xr3:uid="{5DE5B11F-E841-CF41-9C74-5610B20C99F1}" name="map_scale"/>
-    <tableColumn id="48" xr3:uid="{79A194EF-E679-C24C-BE38-E97569E976AA}" name="map_max_sample"/>
-    <tableColumn id="49" xr3:uid="{A0BE4E97-52EA-C245-B384-C2C954FDB62B}" name="map_margin"/>
-    <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s"/>
-    <tableColumn id="12" xr3:uid="{A646D821-0BC3-7144-9611-00F929630647}" name="prob_map_s_calib"/>
-    <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr"/>
-    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust"/>
-    <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon"/>
-    <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="8"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="7"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="2"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
-    <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
-    <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
-    <tableColumn id="33" xr3:uid="{FE34BCA4-242F-3342-9900-5E0B6676722C}" name="wing_span"/>
-    <tableColumn id="27" xr3:uid="{EFA82C59-4775-1545-BF9E-65F94819FAF1}" name="color"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AK8" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:AK8" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+  <tableColumns count="37">
+    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="37" dataCellStyle="Normal_Feuil1"/>
+    <tableColumn id="14" xr3:uid="{B5129423-DA1B-1C48-BC9F-C35BC25D47A1}" name="keep" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{0668329D-3607-7843-896E-E19145D713AC}" name="multisensor" dataDxfId="0"/>
+    <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start" dataDxfId="1"/>
+    <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="35"/>
+    <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N" dataDxfId="34"/>
+    <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W" dataDxfId="33"/>
+    <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S" dataDxfId="32"/>
+    <tableColumn id="46" xr3:uid="{4736E547-D326-6746-9382-CDD964418C71}" name="extent_E" dataDxfId="31"/>
+    <tableColumn id="47" xr3:uid="{5DE5B11F-E841-CF41-9C74-5610B20C99F1}" name="map_scale" dataDxfId="30"/>
+    <tableColumn id="48" xr3:uid="{79A194EF-E679-C24C-BE38-E97569E976AA}" name="map_max_sample" dataDxfId="29"/>
+    <tableColumn id="49" xr3:uid="{A0BE4E97-52EA-C245-B384-C2C954FDB62B}" name="map_margin" dataDxfId="28"/>
+    <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{A646D821-0BC3-7144-9611-00F929630647}" name="prob_map_s_calib" dataDxfId="26"/>
+    <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr" dataDxfId="25"/>
+    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat" dataDxfId="21"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="20"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="19"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="18"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="17"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="16"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="10"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name" dataDxfId="7"/>
+    <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass" dataDxfId="6"/>
+    <tableColumn id="33" xr3:uid="{FE34BCA4-242F-3342-9900-5E0B6676722C}" name="wing_span" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{EFA82C59-4775-1545-BF9E-65F94819FAF1}" name="color" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1133,227 +1461,841 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AK13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1640625" customWidth="1"/>
-    <col min="22" max="22" width="14.1640625" customWidth="1"/>
-    <col min="23" max="29" width="17.33203125" customWidth="1"/>
-    <col min="31" max="31" width="17.33203125" customWidth="1"/>
-    <col min="32" max="32" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5" customWidth="1"/>
-    <col min="39" max="39" width="16.33203125" customWidth="1"/>
-    <col min="45" max="47" width="15.1640625" customWidth="1"/>
-    <col min="48" max="48" width="14.5" customWidth="1"/>
-    <col min="49" max="49" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="18" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" customWidth="1"/>
+    <col min="24" max="24" width="14.1640625" customWidth="1"/>
+    <col min="25" max="31" width="17.33203125" customWidth="1"/>
+    <col min="33" max="33" width="17.33203125" customWidth="1"/>
+    <col min="34" max="34" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5" customWidth="1"/>
+    <col min="41" max="41" width="16.33203125" customWidth="1"/>
+    <col min="47" max="49" width="15.1640625" customWidth="1"/>
+    <col min="50" max="50" width="14.5" customWidth="1"/>
+    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AE1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44063</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44357</v>
+      </c>
+      <c r="F2" s="4">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="G2" s="2">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="H2" s="5">
+        <v>29</v>
+      </c>
+      <c r="I2" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J2" s="2">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>300</v>
+      </c>
+      <c r="M2" s="2">
+        <v>30</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="S2" s="2">
+        <v>39.988903000000001</v>
+      </c>
+      <c r="T2" s="2">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="U2" s="3">
+        <v>44063</v>
+      </c>
+      <c r="V2" s="3">
+        <v>44136</v>
+      </c>
+      <c r="W2" s="3">
+        <v>44324</v>
+      </c>
+      <c r="X2" s="3">
+        <v>44357</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>120</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AE2" s="4">
         <v>15</v>
       </c>
-      <c r="Y1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK2" s="6"/>
+    </row>
+    <row r="3" spans="1:37">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44078</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44406</v>
+      </c>
+      <c r="F3" s="4">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
         <v>29</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="I3" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J3" s="2">
+        <v>48</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>300</v>
+      </c>
+      <c r="M3" s="2">
         <v>30</v>
       </c>
-      <c r="AB1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="S3" s="2">
+        <v>39.988903000000001</v>
+      </c>
+      <c r="T3" s="2">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="U3" s="3">
+        <v>44078</v>
+      </c>
+      <c r="V3" s="3">
+        <v>44228</v>
+      </c>
+      <c r="W3" s="3">
+        <v>44404</v>
+      </c>
+      <c r="X3" s="3">
+        <v>44406</v>
+      </c>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>120</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>100</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>15</v>
+      </c>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK3" s="2"/>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="4">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5">
+        <v>29</v>
+      </c>
+      <c r="I4" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J4" s="2">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2">
         <v>2</v>
       </c>
-      <c r="AF1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="L4" s="2">
+        <v>300</v>
+      </c>
+      <c r="M4" s="2">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q4" s="2">
         <v>0</v>
       </c>
-      <c r="AH1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="R4" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="S4" s="2">
+        <v>39.988903000000001</v>
+      </c>
+      <c r="T4" s="2">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>120</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>100</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="AJ4" s="2">
         <v>35</v>
       </c>
+      <c r="AK4" s="2"/>
     </row>
-    <row r="2" spans="1:35">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1">
-        <v>42906</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43222</v>
-      </c>
-      <c r="D2" s="4">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>-16</v>
-      </c>
-      <c r="G2">
+    <row r="5" spans="1:37">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>23</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
+      <c r="C5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="4">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5">
+        <v>29</v>
+      </c>
+      <c r="I5" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J5" s="2">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
         <v>300</v>
       </c>
-      <c r="K2">
+      <c r="M5" s="2">
         <v>30</v>
       </c>
-      <c r="L2">
+      <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
         <v>0.9</v>
       </c>
-      <c r="O2">
+      <c r="Q5" s="2">
         <v>0</v>
       </c>
-      <c r="P2">
+      <c r="R5" s="2">
         <v>1.4</v>
       </c>
-      <c r="Q2">
-        <v>17.05</v>
-      </c>
-      <c r="R2">
-        <v>48.9</v>
-      </c>
-      <c r="S2" s="1">
-        <v>42906</v>
-      </c>
-      <c r="T2" s="1">
-        <v>42952</v>
-      </c>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="4">
+      <c r="S5" s="2">
+        <v>39.988903000000001</v>
+      </c>
+      <c r="T5" s="2">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="4">
         <v>0.1</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="AB5" s="4">
         <v>0.9</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AC5" s="4">
         <v>120</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AD5" s="4">
         <v>100</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AE5" s="4">
         <v>15</v>
       </c>
-      <c r="AF2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI2" s="2"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>28.9</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK5" s="2"/>
     </row>
-    <row r="8" spans="1:35">
-      <c r="R8" s="3"/>
+    <row r="6" spans="1:37">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>43983</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44469</v>
+      </c>
+      <c r="F6" s="4">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6</v>
+      </c>
+      <c r="H6" s="5">
+        <v>29</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J6" s="2">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>300</v>
+      </c>
+      <c r="M6" s="2">
+        <v>30</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="S6" s="2">
+        <v>39.988903000000001</v>
+      </c>
+      <c r="T6" s="2">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="U6" s="3">
+        <v>43983</v>
+      </c>
+      <c r="V6" s="3">
+        <v>44146</v>
+      </c>
+      <c r="W6" s="3">
+        <v>44333</v>
+      </c>
+      <c r="X6" s="3">
+        <v>44469</v>
+      </c>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>120</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>100</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>15</v>
+      </c>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>31.8</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK6" s="2"/>
     </row>
-    <row r="13" spans="1:35">
-      <c r="H13" s="5"/>
+    <row r="7" spans="1:37">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44020</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44393</v>
+      </c>
+      <c r="F7" s="4">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5">
+        <v>29</v>
+      </c>
+      <c r="I7" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J7" s="2">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>300</v>
+      </c>
+      <c r="M7" s="2">
+        <v>30</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="S7" s="2">
+        <v>39.971646999999997</v>
+      </c>
+      <c r="T7" s="2">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="U7" s="3">
+        <v>44020</v>
+      </c>
+      <c r="V7" s="3">
+        <v>44147</v>
+      </c>
+      <c r="W7" s="3">
+        <v>44294</v>
+      </c>
+      <c r="X7" s="3">
+        <v>44393</v>
+      </c>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AC7" s="4">
+        <v>120</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>100</v>
+      </c>
+      <c r="AE7" s="4">
+        <v>15</v>
+      </c>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK7" s="2"/>
+    </row>
+    <row r="8" spans="1:37">
+      <c r="A8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>44012</v>
+      </c>
+      <c r="E8" s="3">
+        <v>44399</v>
+      </c>
+      <c r="F8" s="4">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6</v>
+      </c>
+      <c r="H8" s="5">
+        <v>29</v>
+      </c>
+      <c r="I8" s="2">
+        <v>-15</v>
+      </c>
+      <c r="J8" s="2">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>300</v>
+      </c>
+      <c r="M8" s="2">
+        <v>30</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="S8" s="2">
+        <v>39.952868000000002</v>
+      </c>
+      <c r="T8" s="2">
+        <v>-3.340795</v>
+      </c>
+      <c r="U8" s="3">
+        <v>44012</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="3">
+        <v>44399</v>
+      </c>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>120</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>100</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ8" s="2">
+        <v>35</v>
+      </c>
+      <c r="AK8" s="2"/>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="J13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
Add 28BP + update index
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Library/CloudStorage/Box-Box/MK-RCRC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78204D2D-8011-8043-9FEB-7FFFE3F62648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B728231-A68A-3344-9D39-EC50FADD144A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="2520" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47200" yWindow="1580" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>mass</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t xml:space="preserve">data stoped 2021-10-03. Just over 1 month of activity and pressure data but no movement/migration. </t>
+  </si>
+  <si>
+    <t>#C95D63</t>
   </si>
 </sst>
 </file>
@@ -815,14 +818,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -1114,6 +1109,14 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1195,45 +1198,48 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AL13" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A1:AL13" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL13">
+    <sortCondition ref="AI1:AI13"/>
+  </sortState>
   <tableColumns count="38">
     <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="37" dataCellStyle="Normal_Feuil1"/>
     <tableColumn id="14" xr3:uid="{B5129423-DA1B-1C48-BC9F-C35BC25D47A1}" name="keep" dataDxfId="36"/>
     <tableColumn id="15" xr3:uid="{0668329D-3607-7843-896E-E19145D713AC}" name="multisensor" dataDxfId="35"/>
-    <tableColumn id="17" xr3:uid="{1C0985E6-0BAC-7C4C-B5C0-7D66F36E357E}" name="description" dataDxfId="0"/>
-    <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start" dataDxfId="34"/>
-    <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="32"/>
-    <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N" dataDxfId="31"/>
-    <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W" dataDxfId="30"/>
-    <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S" dataDxfId="29"/>
-    <tableColumn id="46" xr3:uid="{4736E547-D326-6746-9382-CDD964418C71}" name="extent_E" dataDxfId="28"/>
-    <tableColumn id="47" xr3:uid="{5DE5B11F-E841-CF41-9C74-5610B20C99F1}" name="map_scale" dataDxfId="27"/>
-    <tableColumn id="48" xr3:uid="{79A194EF-E679-C24C-BE38-E97569E976AA}" name="map_max_sample" dataDxfId="26"/>
-    <tableColumn id="49" xr3:uid="{A0BE4E97-52EA-C245-B384-C2C954FDB62B}" name="map_margin" dataDxfId="25"/>
-    <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{A646D821-0BC3-7144-9611-00F929630647}" name="prob_map_s_calib" dataDxfId="23"/>
-    <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr" dataDxfId="22"/>
-    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="14"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="13"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="7"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name" dataDxfId="4"/>
-    <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass" dataDxfId="3"/>
-    <tableColumn id="33" xr3:uid="{FE34BCA4-242F-3342-9900-5E0B6676722C}" name="wing_span" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{D3A9E802-1001-AF49-A5D8-88167423080E}" name="Color" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{1C0985E6-0BAC-7C4C-B5C0-7D66F36E357E}" name="description" dataDxfId="34"/>
+    <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start" dataDxfId="33"/>
+    <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="31"/>
+    <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N" dataDxfId="30"/>
+    <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W" dataDxfId="29"/>
+    <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S" dataDxfId="28"/>
+    <tableColumn id="46" xr3:uid="{4736E547-D326-6746-9382-CDD964418C71}" name="extent_E" dataDxfId="27"/>
+    <tableColumn id="47" xr3:uid="{5DE5B11F-E841-CF41-9C74-5610B20C99F1}" name="map_scale" dataDxfId="26"/>
+    <tableColumn id="48" xr3:uid="{79A194EF-E679-C24C-BE38-E97569E976AA}" name="map_max_sample" dataDxfId="25"/>
+    <tableColumn id="49" xr3:uid="{A0BE4E97-52EA-C245-B384-C2C954FDB62B}" name="map_margin" dataDxfId="24"/>
+    <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{A646D821-0BC3-7144-9611-00F929630647}" name="prob_map_s_calib" dataDxfId="22"/>
+    <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr" dataDxfId="21"/>
+    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="16"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="14"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="13"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="12"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="6"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name" dataDxfId="3"/>
+    <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass" dataDxfId="2"/>
+    <tableColumn id="33" xr3:uid="{FE34BCA4-242F-3342-9900-5E0B6676722C}" name="wing_span" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{D3A9E802-1001-AF49-A5D8-88167423080E}" name="Color" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1539,8 +1545,8 @@
   <dimension ref="A1:AL13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1688,7 +1694,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
@@ -1700,10 +1706,10 @@
         <v>65</v>
       </c>
       <c r="E2" s="2">
-        <v>44063</v>
+        <v>44020</v>
       </c>
       <c r="F2" s="2">
-        <v>44357</v>
+        <v>44393</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
@@ -1743,22 +1749,22 @@
         <v>1.4</v>
       </c>
       <c r="T2" s="1">
-        <v>39.988903000000001</v>
+        <v>39.971646999999997</v>
       </c>
       <c r="U2" s="1">
         <v>-3.3782700000000001</v>
       </c>
       <c r="V2" s="2">
-        <v>44063</v>
+        <v>44020</v>
       </c>
       <c r="W2" s="2">
-        <v>44136</v>
+        <v>44147</v>
       </c>
       <c r="X2" s="2">
-        <v>44324</v>
+        <v>44294</v>
       </c>
       <c r="Y2" s="2">
-        <v>44357</v>
+        <v>44393</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
@@ -1777,39 +1783,41 @@
       <c r="AF2" s="3">
         <v>15</v>
       </c>
-      <c r="AG2" s="1"/>
+      <c r="AG2" s="2"/>
       <c r="AH2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AJ2" s="1">
-        <v>34.200000000000003</v>
+        <v>60.4</v>
       </c>
       <c r="AK2" s="1">
         <v>35</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E3" s="2">
-        <v>44078</v>
+        <v>44012</v>
       </c>
       <c r="F3" s="2">
-        <v>44406</v>
+        <v>44399</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -1849,22 +1857,18 @@
         <v>1.4</v>
       </c>
       <c r="T3" s="1">
-        <v>39.988903000000001</v>
+        <v>39.952868000000002</v>
       </c>
       <c r="U3" s="1">
-        <v>-3.3782700000000001</v>
+        <v>-3.340795</v>
       </c>
       <c r="V3" s="2">
-        <v>44078</v>
-      </c>
-      <c r="W3" s="2">
-        <v>44228</v>
-      </c>
-      <c r="X3" s="2">
-        <v>44404</v>
-      </c>
+        <v>44012</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
       <c r="Y3" s="2">
-        <v>44406</v>
+        <v>44399</v>
       </c>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
@@ -1885,13 +1889,13 @@
       </c>
       <c r="AG3" s="2"/>
       <c r="AH3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AJ3" s="1">
-        <v>31.2</v>
+        <v>60</v>
       </c>
       <c r="AK3" s="1">
         <v>35</v>
@@ -1900,17 +1904,23 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="8">
+        <v>44426</v>
+      </c>
+      <c r="F4" s="8">
+        <v>44742</v>
+      </c>
       <c r="G4" s="3">
         <v>0</v>
       </c>
@@ -1948,16 +1958,24 @@
       <c r="S4" s="1">
         <v>1.4</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4">
         <v>39.988903000000001</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4">
         <v>-3.3782700000000001</v>
       </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
+      <c r="V4" s="8">
+        <v>44426</v>
+      </c>
+      <c r="W4" s="2">
+        <v>44536</v>
+      </c>
+      <c r="X4" s="2">
+        <v>44681</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>44742</v>
+      </c>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="3">
@@ -1975,34 +1993,40 @@
       <c r="AF4" s="3">
         <v>15</v>
       </c>
-      <c r="AG4" s="2"/>
+      <c r="AG4" t="s">
+        <v>54</v>
+      </c>
       <c r="AH4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ4" s="1">
-        <v>32.1</v>
-      </c>
-      <c r="AK4" s="1">
-        <v>35</v>
-      </c>
-      <c r="AL4" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="8">
+        <v>44404</v>
+      </c>
+      <c r="F5" s="8">
+        <v>44756</v>
+      </c>
       <c r="G5" s="3">
         <v>0</v>
       </c>
@@ -2040,18 +2064,26 @@
       <c r="S5" s="1">
         <v>1.4</v>
       </c>
-      <c r="T5" s="1">
-        <v>39.988903000000001</v>
-      </c>
-      <c r="U5" s="1">
-        <v>-3.3782700000000001</v>
-      </c>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
+      <c r="T5">
+        <v>39.947544999999998</v>
+      </c>
+      <c r="U5">
+        <v>-3.3407390000000001</v>
+      </c>
+      <c r="V5" s="8">
+        <v>44404</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="8">
+        <v>44756</v>
+      </c>
+      <c r="Z5">
+        <v>39.950184</v>
+      </c>
+      <c r="AA5">
+        <v>-3.3391920000000002</v>
+      </c>
       <c r="AB5" s="3">
         <v>0.09</v>
       </c>
@@ -2067,24 +2099,22 @@
       <c r="AF5" s="3">
         <v>15</v>
       </c>
-      <c r="AG5" s="2"/>
+      <c r="AG5" t="s">
+        <v>55</v>
+      </c>
       <c r="AH5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ5" s="1">
-        <v>28.9</v>
-      </c>
-      <c r="AK5" s="1">
-        <v>35</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>0</v>
@@ -2093,13 +2123,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="2">
-        <v>43983</v>
-      </c>
-      <c r="F6" s="2">
-        <v>44469</v>
+        <v>68</v>
+      </c>
+      <c r="E6" s="8">
+        <v>44395</v>
+      </c>
+      <c r="F6" s="8">
+        <v>44778</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -2138,23 +2168,19 @@
       <c r="S6" s="1">
         <v>1.4</v>
       </c>
-      <c r="T6" s="1">
-        <v>39.988903000000001</v>
-      </c>
-      <c r="U6" s="1">
-        <v>-3.3782700000000001</v>
-      </c>
-      <c r="V6" s="2">
-        <v>43983</v>
-      </c>
-      <c r="W6" s="2">
-        <v>44146</v>
-      </c>
-      <c r="X6" s="2">
-        <v>44333</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>44469</v>
+      <c r="T6">
+        <v>39.947809999999997</v>
+      </c>
+      <c r="U6">
+        <v>-3.3501799999999999</v>
+      </c>
+      <c r="V6" s="8">
+        <v>44395</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="8">
+        <v>44778</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
@@ -2173,24 +2199,22 @@
       <c r="AF6" s="3">
         <v>15</v>
       </c>
-      <c r="AG6" s="2"/>
+      <c r="AG6" t="s">
+        <v>56</v>
+      </c>
       <c r="AH6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ6" s="1">
-        <v>31.8</v>
-      </c>
-      <c r="AK6" s="1">
-        <v>35</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>1</v>
@@ -2202,10 +2226,10 @@
         <v>65</v>
       </c>
       <c r="E7" s="2">
-        <v>44020</v>
+        <v>44063</v>
       </c>
       <c r="F7" s="2">
-        <v>44393</v>
+        <v>44357</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -2245,22 +2269,22 @@
         <v>1.4</v>
       </c>
       <c r="T7" s="1">
-        <v>39.971646999999997</v>
+        <v>39.988903000000001</v>
       </c>
       <c r="U7" s="1">
         <v>-3.3782700000000001</v>
       </c>
       <c r="V7" s="2">
-        <v>44020</v>
+        <v>44063</v>
       </c>
       <c r="W7" s="2">
-        <v>44147</v>
+        <v>44136</v>
       </c>
       <c r="X7" s="2">
-        <v>44294</v>
+        <v>44324</v>
       </c>
       <c r="Y7" s="2">
-        <v>44393</v>
+        <v>44357</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -2279,41 +2303,39 @@
       <c r="AF7" s="3">
         <v>15</v>
       </c>
-      <c r="AG7" s="2"/>
+      <c r="AG7" s="1"/>
       <c r="AH7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ7" s="1">
-        <v>60.4</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="AK7" s="1">
         <v>35</v>
       </c>
       <c r="AL7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="2">
-        <v>44012</v>
+        <v>44078</v>
       </c>
       <c r="F8" s="2">
-        <v>44399</v>
+        <v>44406</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -2353,18 +2375,22 @@
         <v>1.4</v>
       </c>
       <c r="T8" s="1">
-        <v>39.952868000000002</v>
+        <v>39.988903000000001</v>
       </c>
       <c r="U8" s="1">
-        <v>-3.340795</v>
+        <v>-3.3782700000000001</v>
       </c>
       <c r="V8" s="2">
-        <v>44012</v>
-      </c>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
+        <v>44078</v>
+      </c>
+      <c r="W8" s="2">
+        <v>44228</v>
+      </c>
+      <c r="X8" s="2">
+        <v>44404</v>
+      </c>
       <c r="Y8" s="2">
-        <v>44399</v>
+        <v>44406</v>
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
@@ -2385,13 +2411,13 @@
       </c>
       <c r="AG8" s="2"/>
       <c r="AH8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ8" s="1">
-        <v>60</v>
+        <v>31.2</v>
       </c>
       <c r="AK8" s="1">
         <v>35</v>
@@ -2400,23 +2426,17 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="8">
-        <v>44426</v>
-      </c>
-      <c r="F9" s="8">
-        <v>44733</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="3">
         <v>0</v>
       </c>
@@ -2454,24 +2474,16 @@
       <c r="S9" s="1">
         <v>1.4</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="1">
         <v>39.988903000000001</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="1">
         <v>-3.3782700000000001</v>
       </c>
-      <c r="V9" s="8">
-        <v>44426</v>
-      </c>
-      <c r="W9" s="2">
-        <v>44538</v>
-      </c>
-      <c r="X9" s="2">
-        <v>44713</v>
-      </c>
-      <c r="Y9" s="8">
-        <v>44733</v>
-      </c>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="3">
@@ -2489,40 +2501,34 @@
       <c r="AF9" s="3">
         <v>15</v>
       </c>
-      <c r="AG9" t="s">
-        <v>53</v>
-      </c>
+      <c r="AG9" s="2"/>
       <c r="AH9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="AI9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ9" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL9" s="1"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="8">
-        <v>44426</v>
-      </c>
-      <c r="F10" s="8">
-        <v>44742</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="3">
         <v>0</v>
       </c>
@@ -2560,24 +2566,16 @@
       <c r="S10" s="1">
         <v>1.4</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="1">
         <v>39.988903000000001</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="1">
         <v>-3.3782700000000001</v>
       </c>
-      <c r="V10" s="8">
-        <v>44426</v>
-      </c>
-      <c r="W10" s="2">
-        <v>44536</v>
-      </c>
-      <c r="X10" s="2">
-        <v>44681</v>
-      </c>
-      <c r="Y10" s="8">
-        <v>44742</v>
-      </c>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="3">
@@ -2595,24 +2593,24 @@
       <c r="AF10" s="3">
         <v>15</v>
       </c>
-      <c r="AG10" t="s">
-        <v>54</v>
-      </c>
+      <c r="AG10" s="2"/>
       <c r="AH10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>28.9</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL10" s="1"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="b">
         <v>0</v>
@@ -2621,13 +2619,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="8">
-        <v>44404</v>
-      </c>
-      <c r="F11" s="8">
-        <v>44756</v>
+        <v>64</v>
+      </c>
+      <c r="E11" s="2">
+        <v>43983</v>
+      </c>
+      <c r="F11" s="2">
+        <v>44469</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -2666,26 +2664,26 @@
       <c r="S11" s="1">
         <v>1.4</v>
       </c>
-      <c r="T11">
-        <v>39.947544999999998</v>
-      </c>
-      <c r="U11">
-        <v>-3.3407390000000001</v>
-      </c>
-      <c r="V11" s="8">
-        <v>44404</v>
-      </c>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="8">
-        <v>44756</v>
-      </c>
-      <c r="Z11">
-        <v>39.950184</v>
-      </c>
-      <c r="AA11">
-        <v>-3.3391920000000002</v>
-      </c>
+      <c r="T11" s="1">
+        <v>39.988903000000001</v>
+      </c>
+      <c r="U11" s="1">
+        <v>-3.3782700000000001</v>
+      </c>
+      <c r="V11" s="2">
+        <v>43983</v>
+      </c>
+      <c r="W11" s="2">
+        <v>44146</v>
+      </c>
+      <c r="X11" s="2">
+        <v>44333</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>44469</v>
+      </c>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
       <c r="AB11" s="3">
         <v>0.09</v>
       </c>
@@ -2701,37 +2699,39 @@
       <c r="AF11" s="3">
         <v>15</v>
       </c>
-      <c r="AG11" t="s">
-        <v>55</v>
-      </c>
+      <c r="AG11" s="2"/>
       <c r="AH11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>35</v>
+      </c>
       <c r="AL11" s="1"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="8">
-        <v>44395</v>
+        <v>44426</v>
       </c>
       <c r="F12" s="8">
-        <v>44778</v>
+        <v>44733</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -2771,18 +2771,22 @@
         <v>1.4</v>
       </c>
       <c r="T12">
-        <v>39.947809999999997</v>
+        <v>39.988903000000001</v>
       </c>
       <c r="U12">
-        <v>-3.3501799999999999</v>
+        <v>-3.3782700000000001</v>
       </c>
       <c r="V12" s="8">
-        <v>44395</v>
-      </c>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
+        <v>44426</v>
+      </c>
+      <c r="W12" s="2">
+        <v>44538</v>
+      </c>
+      <c r="X12" s="2">
+        <v>44713</v>
+      </c>
       <c r="Y12" s="8">
-        <v>44778</v>
+        <v>44733</v>
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
@@ -2802,17 +2806,19 @@
         <v>15</v>
       </c>
       <c r="AG12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
+      <c r="AL12" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -2824,7 +2830,9 @@
       <c r="C13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E13" s="8">
         <v>44418</v>
       </c>
@@ -2841,7 +2849,7 @@
         <v>34</v>
       </c>
       <c r="J13" s="1">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="K13" s="1">
         <v>42</v>
@@ -2914,7 +2922,9 @@
       </c>
       <c r="AJ13" s="5"/>
       <c r="AK13" s="5"/>
-      <c r="AL13" s="1"/>
+      <c r="AL13" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>